<commit_message>
POM with updated code
</commit_message>
<xml_diff>
--- a/DemoProject1/TestData/DemoData.xlsx
+++ b/DemoProject1/TestData/DemoData.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAPIL\source\repos\DemoProject1\DemoProject1\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABF68F7-C4C1-4598-87AA-3EA8D4508EBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238AEB06-359B-4CAC-A2A4-17134CB8D063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EmailTemplate" sheetId="1" r:id="rId1"/>
+    <sheet name="WordTemplate" sheetId="2" r:id="rId2"/>
+    <sheet name="ScriptTemplate" sheetId="3" r:id="rId3"/>
+    <sheet name="Category" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,49 +28,115 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Singh</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Recipient</t>
-  </si>
-  <si>
-    <t>Application RCVD date</t>
-  </si>
-  <si>
-    <t>Leave Start Date</t>
-  </si>
-  <si>
-    <t>kapil.kumar@gmail.com</t>
-  </si>
-  <si>
-    <t>4/13/2020</t>
-  </si>
-  <si>
-    <t>4/14/2020</t>
-  </si>
-  <si>
-    <t>David Jhones Test</t>
-  </si>
-  <si>
-    <t>start date</t>
-  </si>
-  <si>
-    <t>end date</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Attachment Container</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Primustest</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>xyz@gmail.com</t>
+  </si>
+  <si>
+    <t>Leave Request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of attachment </t>
+  </si>
+  <si>
+    <t>Devtest</t>
+  </si>
+  <si>
+    <t>Primus Test</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single </t>
+  </si>
+  <si>
+    <t>Divs</t>
+  </si>
+  <si>
+    <t>Primus Test1</t>
+  </si>
+  <si>
+    <t>Envelope</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Primus Test2</t>
+  </si>
+  <si>
+    <t>Document1</t>
+  </si>
+  <si>
+    <t>secondaryCat</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>QAAutomation</t>
+  </si>
+  <si>
+    <t>Script</t>
+  </si>
+  <si>
+    <t>PrimusTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is test template </t>
+  </si>
+  <si>
+    <t>Category Name</t>
+  </si>
+  <si>
+    <t>Primus_test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,19 +152,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,11 +182,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -397,75 +470,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{CAE67BE6-9583-49CF-AE7B-31EC3048FA1C}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{94F23EE6-D824-45AB-B474-A2EDE67A0178}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{EFDF6A3C-3C4E-4F64-9483-CCA74F305E53}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{F6391783-2BA2-4CAA-A2D1-F4F2D0CADCE4}"/>
+    <hyperlink ref="A2" r:id="rId4" display="QAAutomation@291" xr:uid="{B1451AA0-7771-4CDC-9CC0-4042EB504733}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC21B21C-AC20-4740-B672-65621F043E7D}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A830F3-E664-44E5-A7F2-B6A00750D2C9}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EEE90CD-F092-48E6-9B82-A0BE093CC777}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
digital desk code added
</commit_message>
<xml_diff>
--- a/DemoProject1/TestData/DemoData.xlsx
+++ b/DemoProject1/TestData/DemoData.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAPIL\source\repos\DemoProject1\DemoProject1\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DemoProject1\DemoProject1\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238AEB06-359B-4CAC-A2A4-17134CB8D063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946CE5FB-E610-49CE-891B-4A6E3FD97751}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmailTemplate" sheetId="1" r:id="rId1"/>
     <sheet name="WordTemplate" sheetId="2" r:id="rId2"/>
     <sheet name="ScriptTemplate" sheetId="3" r:id="rId3"/>
-    <sheet name="Category" sheetId="4" r:id="rId4"/>
+    <sheet name="Login" sheetId="4" r:id="rId4"/>
+    <sheet name="Manual Claim" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -126,10 +127,112 @@
     <t xml:space="preserve">This is test template </t>
   </si>
   <si>
-    <t>Category Name</t>
-  </si>
-  <si>
-    <t>Primus_test</t>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>vishal.singh@primussoft.com</t>
+  </si>
+  <si>
+    <t>Primus1234$</t>
+  </si>
+  <si>
+    <t>Primus1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loss Date </t>
+  </si>
+  <si>
+    <t>Recieved Date</t>
+  </si>
+  <si>
+    <t>Carrier Name</t>
+  </si>
+  <si>
+    <t>Carrier Ref No#</t>
+  </si>
+  <si>
+    <t>Claim Number</t>
+  </si>
+  <si>
+    <t>Cat Code</t>
+  </si>
+  <si>
+    <t>Peril Type</t>
+  </si>
+  <si>
+    <t>Property Type</t>
+  </si>
+  <si>
+    <t>Claim Source</t>
+  </si>
+  <si>
+    <t>Policy Number</t>
+  </si>
+  <si>
+    <t>Policy Holder's Name</t>
+  </si>
+  <si>
+    <t>Policy Holder's Mobile</t>
+  </si>
+  <si>
+    <t>Policy Holder's Email</t>
+  </si>
+  <si>
+    <t>Address Line 1</t>
+  </si>
+  <si>
+    <t>Address Line 2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>kapil12@mailinator.com</t>
+  </si>
+  <si>
+    <t>4th Avenue</t>
+  </si>
+  <si>
+    <t>new york</t>
+  </si>
+  <si>
+    <t>Onsite Contact Name</t>
+  </si>
+  <si>
+    <t>Onsite Contact Mobile</t>
+  </si>
+  <si>
+    <t>Onsite Contact Email</t>
+  </si>
+  <si>
+    <t>kapil</t>
+  </si>
+  <si>
+    <t>kapil@gmail.com</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>This is test remark</t>
+  </si>
+  <si>
+    <t>DD989438</t>
   </si>
 </sst>
 </file>
@@ -182,13 +285,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -693,15 +802,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EEE90CD-F092-48E6-9B82-A0BE093CC777}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="31.21875" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -710,15 +819,206 @@
         <v>32</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>33</v>
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D4133F0C-33C5-4A94-BEC8-F3382931DFBF}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{4B137C23-EFDB-4A45-B533-03FEFBCC14BD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35C3FB6-8894-44D5-BA07-33C1FA6560B0}">
+  <dimension ref="A1:W4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" customWidth="1"/>
+    <col min="18" max="18" width="10.88671875" customWidth="1"/>
+    <col min="20" max="20" width="14.44140625" customWidth="1"/>
+    <col min="21" max="21" width="17.44140625" customWidth="1"/>
+    <col min="22" max="22" width="18.33203125" customWidth="1"/>
+    <col min="23" max="23" width="16.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>2021</v>
+      </c>
+      <c r="B2" s="6">
+        <v>2021</v>
+      </c>
+      <c r="D2" s="6">
+        <v>808080</v>
+      </c>
+      <c r="E2" s="6">
+        <v>808084</v>
+      </c>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="6">
+        <v>9867543212</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>12345</v>
+      </c>
+      <c r="T2" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="6">
+        <v>9876543212</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>26</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{ABE9F68C-7B80-4C53-9899-82A06B93DB6D}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{6213DBAD-98D9-4431-BD2F-476BB51D59C2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>